<commit_message>
grid_loot | element syetem
</commit_message>
<xml_diff>
--- a/Assets/Resources/cardsdata_Modifier.xlsx
+++ b/Assets/Resources/cardsdata_Modifier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul Demars\Documents\5GD-JeuDeCarteHybride\Assets\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabi\Documents\GitHub\5GD-JeuDeCarteHybride\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98188A7A-1EA3-43D5-BD70-55AD5DC444B0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09650589-6AD6-4CED-A219-D78A8FF29AD1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BA23CEE2-B41B-46CD-B525-12E9CDD839F1}"/>
+    <workbookView xWindow="885" yWindow="-120" windowWidth="28035" windowHeight="16440" xr2:uid="{BA23CEE2-B41B-46CD-B525-12E9CDD839F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Classeur1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="86">
   <si>
     <t>ID</t>
   </si>
@@ -45,9 +45,6 @@
     <t>ARMOR</t>
   </si>
   <si>
-    <t>SPECIALSTAT</t>
-  </si>
-  <si>
     <t>1.1</t>
   </si>
   <si>
@@ -277,6 +274,21 @@
   </si>
   <si>
     <t>31.1</t>
+  </si>
+  <si>
+    <t>DAMAGE ELEMENT</t>
+  </si>
+  <si>
+    <t>ARMOR ELEMENT</t>
+  </si>
+  <si>
+    <t>fire</t>
+  </si>
+  <si>
+    <t>ice</t>
+  </si>
+  <si>
+    <t>electric</t>
   </si>
 </sst>
 </file>
@@ -629,18 +641,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F42FD53-3765-4F2B-AA75-4398E65CF0BD}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21:F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -654,141 +668,198 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>42</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>44</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>45</v>
       </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>46</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>47</v>
       </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>48</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>49</v>
       </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>50</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>51</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -796,13 +867,19 @@
       <c r="D11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -810,13 +887,19 @@
       <c r="D12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -824,13 +907,19 @@
       <c r="D13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -838,13 +927,19 @@
       <c r="D14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15">
         <v>6</v>
@@ -852,13 +947,19 @@
       <c r="D15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16">
         <v>6</v>
@@ -866,13 +967,19 @@
       <c r="D16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -880,313 +987,451 @@
       <c r="D17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
         <v>58</v>
       </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>60</v>
       </c>
-      <c r="C19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>61</v>
       </c>
-      <c r="C20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>24</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>62</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>25</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>63</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>64</v>
       </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>65</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>66</v>
       </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>29</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>67</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>30</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>68</v>
       </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>31</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>69</v>
       </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>32</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>70</v>
       </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>83</v>
+      </c>
+      <c r="F32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>33</v>
       </c>
-      <c r="B30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>36</v>
       </c>
-      <c r="B31" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" t="s">
-        <v>73</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>75</v>
       </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>37</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>76</v>
       </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>38</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>77</v>
       </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>83</v>
+      </c>
+      <c r="F37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>39</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>78</v>
       </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>40</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>79</v>
       </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" t="s">
-        <v>80</v>
-      </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
         <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FMOD | Mise à jour Excel
</commit_message>
<xml_diff>
--- a/Assets/Resources/cardsdata_Modifier.xlsx
+++ b/Assets/Resources/cardsdata_Modifier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabi\Documents\GitHub\5GD-JeuDeCarteHybride\Assets\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul Demars\Documents\5GD-JeuDeCarteHybride\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09650589-6AD6-4CED-A219-D78A8FF29AD1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816B420B-3A60-4363-9275-AB298CA2B397}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="-120" windowWidth="28035" windowHeight="16440" xr2:uid="{BA23CEE2-B41B-46CD-B525-12E9CDD839F1}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{BA23CEE2-B41B-46CD-B525-12E9CDD839F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Classeur1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -156,123 +156,15 @@
     <t>38.1</t>
   </si>
   <si>
-    <t>Saggaie</t>
-  </si>
-  <si>
     <t>Gourdin</t>
   </si>
   <si>
-    <t>Baton affuté</t>
-  </si>
-  <si>
-    <t>Marteau en silex</t>
-  </si>
-  <si>
-    <t>épee primitive</t>
-  </si>
-  <si>
-    <t>Lance sauvage</t>
-  </si>
-  <si>
     <t>Sarbacane</t>
   </si>
   <si>
-    <t>Lance pierre</t>
-  </si>
-  <si>
-    <t>Fouet en liane</t>
-  </si>
-  <si>
-    <t>Arc simple</t>
-  </si>
-  <si>
-    <t>Gourdin Ionique</t>
-  </si>
-  <si>
     <t>Arc laser</t>
   </si>
   <si>
-    <t>Bazoolex/Pistolex</t>
-  </si>
-  <si>
-    <t>Fusarbalète</t>
-  </si>
-  <si>
-    <t>Lance foreuse</t>
-  </si>
-  <si>
-    <t>Double Uzi</t>
-  </si>
-  <si>
-    <t>AK-4000</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Tazer</t>
-  </si>
-  <si>
-    <t>Gatling Maxell</t>
-  </si>
-  <si>
-    <t>Tenue de cuir tannée</t>
-  </si>
-  <si>
-    <t>Armure en cuir clouté</t>
-  </si>
-  <si>
-    <t>Cage en fer</t>
-  </si>
-  <si>
-    <t>Protection en fer rouillé</t>
-  </si>
-  <si>
-    <t>Cuirasse en bois et liane</t>
-  </si>
-  <si>
-    <t>Protection en fourrure</t>
-  </si>
-  <si>
-    <t>Tenue en sac de terre</t>
-  </si>
-  <si>
-    <t>Plaque de métal</t>
-  </si>
-  <si>
-    <t>Plastron en peaux</t>
-  </si>
-  <si>
-    <t>Tenue en os de monstre</t>
-  </si>
-  <si>
-    <t>Cotte de maille</t>
-  </si>
-  <si>
-    <t>Armure de métal poli</t>
-  </si>
-  <si>
-    <t>Protection en pneu</t>
-  </si>
-  <si>
-    <t>Tenue en cuir de monstre</t>
-  </si>
-  <si>
-    <t>Uniforme avec écailles</t>
-  </si>
-  <si>
-    <t>Gilet pare balle</t>
-  </si>
-  <si>
-    <t>Tenue anti émeute</t>
-  </si>
-  <si>
-    <t>Armure de combat</t>
-  </si>
-  <si>
-    <t>Super armure énergétique</t>
-  </si>
-  <si>
     <t>31.1</t>
   </si>
   <si>
@@ -282,13 +174,118 @@
     <t>ARMOR ELEMENT</t>
   </si>
   <si>
-    <t>fire</t>
-  </si>
-  <si>
-    <t>ice</t>
-  </si>
-  <si>
-    <t>electric</t>
+    <t>Arc Primitif</t>
+  </si>
+  <si>
+    <t>Lance-pierre</t>
+  </si>
+  <si>
+    <t>Arc à plasma</t>
+  </si>
+  <si>
+    <t>Gourdin éléctrique</t>
+  </si>
+  <si>
+    <t>Sarbacane éclair</t>
+  </si>
+  <si>
+    <t>Lanceur énergétique</t>
+  </si>
+  <si>
+    <t>Lance à impulsion</t>
+  </si>
+  <si>
+    <t>Massue radion</t>
+  </si>
+  <si>
+    <t>Canon sarbacane</t>
+  </si>
+  <si>
+    <t>Lance-atome</t>
+  </si>
+  <si>
+    <t>Lance thermique</t>
+  </si>
+  <si>
+    <t>Arc à impulsion quantique</t>
+  </si>
+  <si>
+    <t>Marteau à phazon</t>
+  </si>
+  <si>
+    <t>Sarbacane railgun</t>
+  </si>
+  <si>
+    <t>Lanceur multi-spectre</t>
+  </si>
+  <si>
+    <t>Lance turbo penetrateur</t>
+  </si>
+  <si>
+    <t>39.1</t>
+  </si>
+  <si>
+    <t>Armure de fourrure</t>
+  </si>
+  <si>
+    <t>Armure d'écorce et de liane</t>
+  </si>
+  <si>
+    <t>Tenue en cuir</t>
+  </si>
+  <si>
+    <t>Armure en os</t>
+  </si>
+  <si>
+    <t>Tenue en morceaux de monstre</t>
+  </si>
+  <si>
+    <t>Fourrure de gros monstres</t>
+  </si>
+  <si>
+    <t>Armure de chêne métalisé</t>
+  </si>
+  <si>
+    <t>Armure en crâne de monstre</t>
+  </si>
+  <si>
+    <t>Tenue en morceau de robot</t>
+  </si>
+  <si>
+    <t>Armure en fourrure énergétique</t>
+  </si>
+  <si>
+    <t>Armure en cuir tesla</t>
+  </si>
+  <si>
+    <t>Armure en os à ion</t>
+  </si>
+  <si>
+    <t>Armure en morceaux plasmique</t>
+  </si>
+  <si>
+    <t>Tenue en fourrure radioactive</t>
+  </si>
+  <si>
+    <t>Armure en bois à fusion</t>
+  </si>
+  <si>
+    <t>Tenue en cuir à radion</t>
+  </si>
+  <si>
+    <t>Armure en os atomique</t>
+  </si>
+  <si>
+    <t>Armure en partie d'uranium</t>
+  </si>
+  <si>
+    <t>Fourrure de chat quantique</t>
+  </si>
+  <si>
+    <t>Armure ionisé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aventurer: </t>
   </si>
 </sst>
 </file>
@@ -641,20 +638,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F42FD53-3765-4F2B-AA75-4398E65CF0BD}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:F39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -668,98 +665,74 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -767,19 +740,13 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -787,19 +754,13 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -807,19 +768,13 @@
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -827,19 +782,13 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -847,19 +796,13 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11">
         <v>4</v>
@@ -867,19 +810,13 @@
       <c r="D11">
         <v>0</v>
       </c>
-      <c r="E11" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -887,19 +824,13 @@
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -907,19 +838,13 @@
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -927,239 +852,167 @@
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
-      <c r="E15" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C16">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
-      <c r="E16" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C17">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
-      <c r="E17" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
-      <c r="E18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
-      <c r="E19" t="s">
-        <v>83</v>
-      </c>
-      <c r="F19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" t="s">
-        <v>58</v>
+        <v>62</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
-      <c r="E20" t="s">
-        <v>83</v>
-      </c>
-      <c r="F20" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
-        <v>2</v>
-      </c>
-      <c r="E21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>83</v>
-      </c>
-      <c r="F22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>2</v>
-      </c>
-      <c r="E23" t="s">
-        <v>83</v>
-      </c>
-      <c r="F23" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F24" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>2</v>
-      </c>
-      <c r="E25" t="s">
-        <v>83</v>
-      </c>
-      <c r="F25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1167,19 +1020,13 @@
       <c r="D26">
         <v>2</v>
       </c>
-      <c r="E26" t="s">
-        <v>83</v>
-      </c>
-      <c r="F26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1187,19 +1034,13 @@
       <c r="D27">
         <v>2</v>
       </c>
-      <c r="E27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1207,19 +1048,13 @@
       <c r="D28">
         <v>2</v>
       </c>
-      <c r="E28" t="s">
-        <v>83</v>
-      </c>
-      <c r="F28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1227,19 +1062,13 @@
       <c r="D29">
         <v>2</v>
       </c>
-      <c r="E29" t="s">
-        <v>83</v>
-      </c>
-      <c r="F29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1247,191 +1076,299 @@
       <c r="D30">
         <v>2</v>
       </c>
-      <c r="E30" t="s">
-        <v>83</v>
-      </c>
-      <c r="F30" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31">
-        <v>2</v>
-      </c>
-      <c r="E31" t="s">
-        <v>83</v>
-      </c>
-      <c r="F31" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>2</v>
-      </c>
-      <c r="E32" t="s">
-        <v>83</v>
-      </c>
-      <c r="F32" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33">
-        <v>2</v>
-      </c>
-      <c r="E33" t="s">
-        <v>83</v>
-      </c>
-      <c r="F33" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>2</v>
-      </c>
-      <c r="E34" t="s">
-        <v>83</v>
-      </c>
-      <c r="F34" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>2</v>
-      </c>
-      <c r="E35" t="s">
-        <v>83</v>
-      </c>
-      <c r="F35" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>2</v>
-      </c>
-      <c r="E36" t="s">
-        <v>83</v>
-      </c>
-      <c r="F36" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>2</v>
-      </c>
-      <c r="E37" t="s">
-        <v>83</v>
-      </c>
-      <c r="F37" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>2</v>
-      </c>
-      <c r="E38" t="s">
-        <v>83</v>
-      </c>
-      <c r="F38" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <v>2</v>
-      </c>
-      <c r="E39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" t="s">
         <v>83</v>
       </c>
-      <c r="F39" t="s">
-        <v>85</v>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>100</v>
+      </c>
+      <c r="B46" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>101</v>
+      </c>
+      <c r="B47" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>102</v>
+      </c>
+      <c r="B48" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>103</v>
+      </c>
+      <c r="B49" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>104</v>
+      </c>
+      <c r="B50" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>105</v>
+      </c>
+      <c r="B51" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>106</v>
+      </c>
+      <c r="B52" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>107</v>
+      </c>
+      <c r="B53" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>108</v>
+      </c>
+      <c r="B54" t="s">
+        <v>84</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>109</v>
+      </c>
+      <c r="B55" t="s">
+        <v>84</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>110</v>
+      </c>
+      <c r="B56" t="s">
+        <v>84</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FMOD | Debug Fmod
</commit_message>
<xml_diff>
--- a/Assets/Resources/cardsdata_Modifier.xlsx
+++ b/Assets/Resources/cardsdata_Modifier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul Demars\Documents\5GD-JeuDeCarteHybride\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816B420B-3A60-4363-9275-AB298CA2B397}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16217A20-B86C-4022-A77D-6A21242D1473}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{BA23CEE2-B41B-46CD-B525-12E9CDD839F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BA23CEE2-B41B-46CD-B525-12E9CDD839F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Classeur1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="87">
   <si>
     <t>ID</t>
   </si>
@@ -286,16 +286,29 @@
   </si>
   <si>
     <t xml:space="preserve">Aventurer: </t>
+  </si>
+  <si>
+    <t>40.1</t>
+  </si>
+  <si>
+    <t>Lance sauvage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -321,9 +334,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F42FD53-3765-4F2B-AA75-4398E65CF0BD}">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,22 +745,22 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>43</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -760,7 +774,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -774,7 +788,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -788,7 +802,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -802,10 +816,10 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -816,7 +830,7 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -830,7 +844,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -844,7 +858,7 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -858,7 +872,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -872,10 +886,10 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -886,7 +900,7 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17">
         <v>8</v>
@@ -900,7 +914,7 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18">
         <v>8</v>
@@ -914,7 +928,7 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19">
         <v>8</v>
@@ -928,7 +942,7 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20">
         <v>8</v>
@@ -942,13 +956,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -956,7 +970,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -970,7 +984,7 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -984,7 +998,7 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -998,7 +1012,7 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1012,13 +1026,13 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1026,7 +1040,7 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1040,7 +1054,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1054,7 +1068,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1068,7 +1082,7 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1082,13 +1096,13 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1096,7 +1110,7 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1110,7 +1124,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1124,7 +1138,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1138,7 +1152,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1152,13 +1166,13 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1166,7 +1180,7 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1180,7 +1194,7 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1194,7 +1208,7 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1208,7 +1222,7 @@
         <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1217,23 +1231,23 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>100</v>
-      </c>
-      <c r="B46" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B47" t="s">
         <v>84</v>
@@ -1247,7 +1261,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B48" t="s">
         <v>84</v>
@@ -1261,7 +1275,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B49" t="s">
         <v>84</v>
@@ -1275,7 +1289,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B50" t="s">
         <v>84</v>
@@ -1289,7 +1303,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B51" t="s">
         <v>84</v>
@@ -1303,7 +1317,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B52" t="s">
         <v>84</v>
@@ -1317,7 +1331,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B53" t="s">
         <v>84</v>
@@ -1331,7 +1345,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B54" t="s">
         <v>84</v>
@@ -1345,7 +1359,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B55" t="s">
         <v>84</v>
@@ -1359,7 +1373,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B56" t="s">
         <v>84</v>
@@ -1371,7 +1385,22 @@
         <v>0</v>
       </c>
     </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>110</v>
+      </c>
+      <c r="B57" t="s">
+        <v>84</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel Cards ID values
</commit_message>
<xml_diff>
--- a/Assets/Resources/cardsdata_Modifier.xlsx
+++ b/Assets/Resources/cardsdata_Modifier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\5GD-JeuDeCarteHybride\Assets\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Logan\Documents\5GD-JeuDeCarteHybride\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A11792-FCEC-4C42-A7CC-534F8A37133A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0B0CBA-BC34-4E7B-B111-D7B5C941B05F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-252" yWindow="-252" windowWidth="23544" windowHeight="12864" xr2:uid="{BA23CEE2-B41B-46CD-B525-12E9CDD839F1}"/>
+    <workbookView xWindow="2940" yWindow="225" windowWidth="21600" windowHeight="11385" xr2:uid="{BA23CEE2-B41B-46CD-B525-12E9CDD839F1}"/>
   </bookViews>
   <sheets>
     <sheet name="cardsdata" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="162">
   <si>
     <t>ID</t>
   </si>
@@ -136,33 +136,9 @@
     <t>32.1</t>
   </si>
   <si>
-    <t>33.1</t>
-  </si>
-  <si>
     <t>30.1</t>
   </si>
   <si>
-    <t>34.1</t>
-  </si>
-  <si>
-    <t>35.1</t>
-  </si>
-  <si>
-    <t>36.1</t>
-  </si>
-  <si>
-    <t>37.1</t>
-  </si>
-  <si>
-    <t>38.1</t>
-  </si>
-  <si>
-    <t>Gourdin</t>
-  </si>
-  <si>
-    <t>Sarbacane</t>
-  </si>
-  <si>
     <t>31.1</t>
   </si>
   <si>
@@ -172,15 +148,6 @@
     <t>ARMOR ELEMENT</t>
   </si>
   <si>
-    <t>Lance-pierre</t>
-  </si>
-  <si>
-    <t>39.1</t>
-  </si>
-  <si>
-    <t>40.1</t>
-  </si>
-  <si>
     <t>2.2</t>
   </si>
   <si>
@@ -202,27 +169,15 @@
     <t>4.2</t>
   </si>
   <si>
-    <t>Lance-pierre de feu</t>
-  </si>
-  <si>
     <t>4.3</t>
   </si>
   <si>
-    <t>Lance-pierre éléctrique</t>
-  </si>
-  <si>
     <t>5.2</t>
   </si>
   <si>
-    <t>5.3</t>
-  </si>
-  <si>
     <t>7.2</t>
   </si>
   <si>
-    <t>7.3</t>
-  </si>
-  <si>
     <t>9.2</t>
   </si>
   <si>
@@ -280,213 +235,18 @@
     <t>29.3</t>
   </si>
   <si>
-    <t>33.2</t>
-  </si>
-  <si>
     <t>31.2</t>
   </si>
   <si>
-    <t>31.3</t>
-  </si>
-  <si>
     <t>32.2</t>
   </si>
   <si>
-    <t>32.3</t>
-  </si>
-  <si>
-    <t>39.2</t>
-  </si>
-  <si>
-    <t>Arc</t>
-  </si>
-  <si>
-    <t>Arc de feu</t>
-  </si>
-  <si>
-    <t>Arc de glace</t>
-  </si>
-  <si>
-    <t>Lance</t>
-  </si>
-  <si>
-    <t>Lance de glace</t>
-  </si>
-  <si>
-    <t>Lance éléctrique</t>
-  </si>
-  <si>
-    <t>Arc énergetique</t>
-  </si>
-  <si>
     <t>Arc énergétique de feu</t>
   </si>
   <si>
-    <t>Gourdin énergétique</t>
-  </si>
-  <si>
-    <t>Sarbacane énergétique</t>
-  </si>
-  <si>
-    <t>Lance énergétique</t>
-  </si>
-  <si>
-    <t>Lance-pierre énergétique</t>
-  </si>
-  <si>
-    <t>Lance-pierre énergétique de glace</t>
-  </si>
-  <si>
-    <t>Lance énergétique éléctrique</t>
-  </si>
-  <si>
-    <t>Arc plasmique</t>
-  </si>
-  <si>
-    <t>Gourdin plasmique</t>
-  </si>
-  <si>
-    <t>Gourdin plasmique en feu</t>
-  </si>
-  <si>
-    <t>Sarbacane plasmique</t>
-  </si>
-  <si>
     <t>Lance-plasma</t>
   </si>
   <si>
-    <t>Lance-plasma éléctrique</t>
-  </si>
-  <si>
-    <t>Lance plasmique</t>
-  </si>
-  <si>
-    <t>Lance plasmique de glace</t>
-  </si>
-  <si>
-    <t>Arc quantique</t>
-  </si>
-  <si>
-    <t>Gourdin quantique enflammé</t>
-  </si>
-  <si>
-    <t>Sarbacane quantique éléctrique</t>
-  </si>
-  <si>
-    <t>Lance-pierre quantique</t>
-  </si>
-  <si>
-    <t>Lance quantique de glace</t>
-  </si>
-  <si>
-    <t>Fourrure</t>
-  </si>
-  <si>
-    <t>Fourrure en feu</t>
-  </si>
-  <si>
-    <t>Fourrure gelée</t>
-  </si>
-  <si>
-    <t>Veste</t>
-  </si>
-  <si>
-    <t>Armure</t>
-  </si>
-  <si>
-    <t>Armure de glace</t>
-  </si>
-  <si>
-    <t>Armure éléctrique</t>
-  </si>
-  <si>
-    <t>Plastron d'os</t>
-  </si>
-  <si>
-    <t>Casque</t>
-  </si>
-  <si>
-    <t>Casque enflammé</t>
-  </si>
-  <si>
-    <t>Casque éléctrique</t>
-  </si>
-  <si>
-    <t>Fourrure plasmique</t>
-  </si>
-  <si>
-    <t>Fourrure plasmique éléctrique</t>
-  </si>
-  <si>
-    <t>Fourrure plasmique de feu</t>
-  </si>
-  <si>
-    <t>Veste plasmique</t>
-  </si>
-  <si>
-    <t>Veste plasmique de glace</t>
-  </si>
-  <si>
-    <t>Veste plasmique éléctrique</t>
-  </si>
-  <si>
-    <t>Armure plasmique de feu</t>
-  </si>
-  <si>
-    <t>Armure plasmique de glace</t>
-  </si>
-  <si>
-    <t>Plastron d'os plasmique</t>
-  </si>
-  <si>
-    <t>Casque plasmique</t>
-  </si>
-  <si>
-    <t>Casque quantique</t>
-  </si>
-  <si>
-    <t>Plastron d'os quantique de feu</t>
-  </si>
-  <si>
-    <t>Plastron d'os quantique</t>
-  </si>
-  <si>
-    <t>Veste quantique de glace</t>
-  </si>
-  <si>
-    <t>Fourrure quantique</t>
-  </si>
-  <si>
-    <t>Plastron d'os énergétique éléctrique</t>
-  </si>
-  <si>
-    <t>Plastron d'os énergétique de glace</t>
-  </si>
-  <si>
-    <t>Plastron d'os énergétique</t>
-  </si>
-  <si>
-    <t>Armure énergétique de glace</t>
-  </si>
-  <si>
-    <t>Armure énergétique de feu</t>
-  </si>
-  <si>
-    <t>Armure énergétique</t>
-  </si>
-  <si>
-    <t>Veste énergétique</t>
-  </si>
-  <si>
-    <t>Fourrure énergétique éléctrique</t>
-  </si>
-  <si>
-    <t>Fourrure énergétique enflammé</t>
-  </si>
-  <si>
-    <t>Fourrure énergétique</t>
-  </si>
-  <si>
     <t>12.2</t>
   </si>
   <si>
@@ -496,9 +256,6 @@
     <t>Casque énergétique</t>
   </si>
   <si>
-    <t>Armure quantique éléctrique</t>
-  </si>
-  <si>
     <t>Aventurer: 1</t>
   </si>
   <si>
@@ -530,13 +287,244 @@
   </si>
   <si>
     <t>Aventurer: 11</t>
+  </si>
+  <si>
+    <t>Arc de fortune de feu</t>
+  </si>
+  <si>
+    <t>Arc de fortune de glace</t>
+  </si>
+  <si>
+    <t>Arc de fortune</t>
+  </si>
+  <si>
+    <t>Arc amélioré</t>
+  </si>
+  <si>
+    <t>Arc amélioré de feu</t>
+  </si>
+  <si>
+    <t>Arc puissant</t>
+  </si>
+  <si>
+    <t>Arc puissant de feu</t>
+  </si>
+  <si>
+    <t>Arc énergétique</t>
+  </si>
+  <si>
+    <t>Lance de fortune de foudre</t>
+  </si>
+  <si>
+    <t>Lance de fortune</t>
+  </si>
+  <si>
+    <t>Lance améliorée</t>
+  </si>
+  <si>
+    <t>Lance améliorée de foudre</t>
+  </si>
+  <si>
+    <t>Lance puissante de foudre</t>
+  </si>
+  <si>
+    <t>Lance puissante</t>
+  </si>
+  <si>
+    <t>Lance énergétique de foudre</t>
+  </si>
+  <si>
+    <t>Lance-pierre de fortune de glace</t>
+  </si>
+  <si>
+    <t>Lance-pierre de fortune</t>
+  </si>
+  <si>
+    <t>Lance-pierre amélioré</t>
+  </si>
+  <si>
+    <t>Lance-pierre amélioré de glace</t>
+  </si>
+  <si>
+    <t>Lance-pierre puissant</t>
+  </si>
+  <si>
+    <t>Lance-pierre de glace</t>
+  </si>
+  <si>
+    <t>Lance thermique de glace</t>
+  </si>
+  <si>
+    <t>Gourdin de fortune de foudre</t>
+  </si>
+  <si>
+    <t>Gourdin de fortune</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>Barre-belée</t>
+  </si>
+  <si>
+    <t>Masse propulsée</t>
+  </si>
+  <si>
+    <t>Marteau énergétique</t>
+  </si>
+  <si>
+    <t>Sarbacane améliorée</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>Sarbacane de fortune de feu</t>
+  </si>
+  <si>
+    <t>Sarbacane de fortune</t>
+  </si>
+  <si>
+    <t>Sarbacane puissante</t>
+  </si>
+  <si>
+    <t>21.4</t>
+  </si>
+  <si>
+    <t>22.2</t>
+  </si>
+  <si>
+    <t>22.3</t>
+  </si>
+  <si>
+    <t>22.4</t>
+  </si>
+  <si>
+    <t>23.4</t>
+  </si>
+  <si>
+    <t>24.3</t>
+  </si>
+  <si>
+    <t>24.4</t>
+  </si>
+  <si>
+    <t>25.4</t>
+  </si>
+  <si>
+    <t>26.4</t>
+  </si>
+  <si>
+    <t>27.3</t>
+  </si>
+  <si>
+    <t>27.4</t>
+  </si>
+  <si>
+    <t>30.2</t>
+  </si>
+  <si>
+    <t>Bouclier de survie de foudre</t>
+  </si>
+  <si>
+    <t>Bouclier de survie de glace</t>
+  </si>
+  <si>
+    <t>Bouclier de survie</t>
+  </si>
+  <si>
+    <t>Casque amélioré</t>
+  </si>
+  <si>
+    <t>Casque amélioré de glace</t>
+  </si>
+  <si>
+    <t>Casque amélioré de feu</t>
+  </si>
+  <si>
+    <t>Casque de fortune de glace</t>
+  </si>
+  <si>
+    <t>Casque de fortune de feu</t>
+  </si>
+  <si>
+    <t>Casque de fortune</t>
+  </si>
+  <si>
+    <t>Plastron de fortune de foudre</t>
+  </si>
+  <si>
+    <t>Plastron de fortune de feu</t>
+  </si>
+  <si>
+    <t>Plastron de fortune</t>
+  </si>
+  <si>
+    <t>Bouclier amélioré</t>
+  </si>
+  <si>
+    <t>Bouclier amélioré de foudre</t>
+  </si>
+  <si>
+    <t>Bouclier amélioré de glace</t>
+  </si>
+  <si>
+    <t>Plastron amélioré</t>
+  </si>
+  <si>
+    <t>Plastron amélioré de foudre</t>
+  </si>
+  <si>
+    <t>Plastron amélioré de feu</t>
+  </si>
+  <si>
+    <t>Bouclier renforcé</t>
+  </si>
+  <si>
+    <t>Bouclier renforcé de foudre</t>
+  </si>
+  <si>
+    <t>Bouclier renforcé de glace</t>
+  </si>
+  <si>
+    <t>Casque renforcé</t>
+  </si>
+  <si>
+    <t>Casque renforcé de glace</t>
+  </si>
+  <si>
+    <t>Casque renforcé de feu</t>
+  </si>
+  <si>
+    <t>Plastron renforcé</t>
+  </si>
+  <si>
+    <t>Plastron renforcé de foudre</t>
+  </si>
+  <si>
+    <t>Plastron renforcé de feu</t>
+  </si>
+  <si>
+    <t>Bouclier énergétique</t>
+  </si>
+  <si>
+    <t>Bouclier thermique de glace</t>
+  </si>
+  <si>
+    <t>Casque énergétique de feu</t>
+  </si>
+  <si>
+    <t>Plastron énergétique</t>
+  </si>
+  <si>
+    <t>Plastron énergétique de foudre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,6 +535,18 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -578,11 +578,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -899,18 +900,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F42FD53-3765-4F2B-AA75-4398E65CF0BD}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="39.5546875" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -924,18 +925,18 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -943,13 +944,16 @@
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -958,15 +962,15 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -974,30 +978,30 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
         <v>41</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1006,105 +1010,105 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
         <v>42</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="B13" s="2" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1112,16 +1116,13 @@
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1130,12 +1131,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1144,15 +1145,15 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1161,12 +1162,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1175,12 +1176,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>96</v>
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>110</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1189,12 +1190,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>109</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1203,12 +1204,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1217,12 +1218,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1231,15 +1232,15 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1248,12 +1249,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -1262,15 +1263,15 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="C24">
         <v>4</v>
@@ -1279,12 +1280,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -1293,12 +1294,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>151</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C26">
         <v>4</v>
@@ -1307,15 +1308,15 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -1324,12 +1325,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C28">
         <v>4</v>
@@ -1337,13 +1338,16 @@
       <c r="D28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C29">
         <v>4</v>
@@ -1351,16 +1355,13 @@
       <c r="D29">
         <v>0</v>
       </c>
-      <c r="E29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -1369,12 +1370,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C31">
         <v>4</v>
@@ -1383,15 +1384,15 @@
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C32">
         <v>8</v>
@@ -1400,12 +1401,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="C33">
         <v>8</v>
@@ -1413,13 +1414,16 @@
       <c r="D33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="C34">
         <v>8</v>
@@ -1427,16 +1431,13 @@
       <c r="D34">
         <v>0</v>
       </c>
-      <c r="E34" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
-      <c r="B35" t="s">
-        <v>112</v>
+      <c r="B35" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="C35">
         <v>8</v>
@@ -1445,15 +1446,15 @@
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
       <c r="B36" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C36">
         <v>8</v>
@@ -1462,12 +1463,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
       <c r="B37" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C37">
         <v>8</v>
@@ -1476,15 +1477,15 @@
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>24</v>
       </c>
       <c r="B39" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1492,13 +1493,16 @@
       <c r="D39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1507,15 +1511,15 @@
         <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1523,154 +1527,151 @@
       <c r="D41">
         <v>1</v>
       </c>
-      <c r="F41" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" t="s">
+        <v>132</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>25</v>
       </c>
-      <c r="B42" t="s">
-        <v>118</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" t="s">
+        <v>138</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>26</v>
       </c>
-      <c r="B43" t="s">
-        <v>119</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>72</v>
-      </c>
-      <c r="B44" t="s">
-        <v>120</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="F44" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>73</v>
-      </c>
-      <c r="B45" t="s">
-        <v>121</v>
-      </c>
-      <c r="C45">
-        <v>0</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="F45" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="B47" t="s">
+        <v>139</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" t="s">
+        <v>141</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" t="s">
+        <v>141</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>27</v>
       </c>
-      <c r="B46" t="s">
-        <v>122</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>75</v>
-      </c>
-      <c r="B47" t="s">
-        <v>122</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>28</v>
-      </c>
-      <c r="B48" t="s">
-        <v>123</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>70</v>
-      </c>
-      <c r="B49" t="s">
-        <v>124</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="F49" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>71</v>
-      </c>
-      <c r="B50" t="s">
-        <v>125</v>
-      </c>
-      <c r="C50">
-        <v>0</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="F50" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>29</v>
-      </c>
       <c r="B51" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1679,12 +1680,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B52" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -1692,16 +1693,13 @@
       <c r="D52">
         <v>2</v>
       </c>
-      <c r="F52" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>123</v>
       </c>
       <c r="B53" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -1710,15 +1708,15 @@
         <v>2</v>
       </c>
       <c r="F53" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="B54" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -1726,13 +1724,16 @@
       <c r="D54">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F54" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>152</v>
+        <v>28</v>
       </c>
       <c r="B55" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -1741,12 +1742,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -1755,12 +1756,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1769,15 +1770,15 @@
         <v>2</v>
       </c>
       <c r="F57" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>79</v>
+        <v>125</v>
       </c>
       <c r="B58" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1786,15 +1787,15 @@
         <v>2</v>
       </c>
       <c r="F58" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1803,12 +1804,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1816,16 +1817,13 @@
       <c r="D60">
         <v>2</v>
       </c>
-      <c r="F60" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1834,15 +1832,15 @@
         <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>35</v>
+        <v>126</v>
       </c>
       <c r="B62" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1850,13 +1848,16 @@
       <c r="D62">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F62" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B63" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1865,12 +1866,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B64" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1878,16 +1879,13 @@
       <c r="D64">
         <v>4</v>
       </c>
-      <c r="F64" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>84</v>
+        <v>127</v>
       </c>
       <c r="B65" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1896,15 +1894,15 @@
         <v>4</v>
       </c>
       <c r="F65" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B66" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1912,13 +1910,16 @@
       <c r="D66">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F66" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="B67" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -1926,16 +1927,13 @@
       <c r="D67">
         <v>4</v>
       </c>
-      <c r="F67" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B68" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -1944,15 +1942,15 @@
         <v>4</v>
       </c>
       <c r="F68" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B69" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -1961,15 +1959,15 @@
         <v>4</v>
       </c>
       <c r="F69" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="B70" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -1977,16 +1975,13 @@
       <c r="D70">
         <v>4</v>
       </c>
-      <c r="F70" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="B71" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -1994,13 +1989,16 @@
       <c r="D71">
         <v>4</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F71" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="B72" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -2008,13 +2006,16 @@
       <c r="D72">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F72" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B73" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -2023,12 +2024,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="B74" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -2037,15 +2038,15 @@
         <v>8</v>
       </c>
       <c r="F74" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B75" t="s">
-        <v>154</v>
+        <v>73</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -2053,16 +2054,13 @@
       <c r="D75">
         <v>8</v>
       </c>
-      <c r="F75" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="B76" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -2070,13 +2068,16 @@
       <c r="D76">
         <v>8</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F76" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>87</v>
+        <v>33</v>
       </c>
       <c r="B77" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -2084,16 +2085,13 @@
       <c r="D77">
         <v>8</v>
       </c>
-      <c r="F77" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="B78" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -2101,13 +2099,16 @@
       <c r="D78">
         <v>8</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F78" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>100</v>
       </c>
       <c r="B84" t="s">
-        <v>155</v>
+        <v>74</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -2116,12 +2117,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>101</v>
       </c>
       <c r="B85" t="s">
-        <v>156</v>
+        <v>75</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -2130,12 +2131,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>102</v>
       </c>
       <c r="B86" t="s">
-        <v>157</v>
+        <v>76</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2144,12 +2145,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>103</v>
       </c>
       <c r="B87" t="s">
-        <v>158</v>
+        <v>77</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2158,12 +2159,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>104</v>
       </c>
       <c r="B88" t="s">
-        <v>159</v>
+        <v>78</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2172,12 +2173,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>105</v>
       </c>
       <c r="B89" t="s">
-        <v>160</v>
+        <v>79</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -2186,12 +2187,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>106</v>
       </c>
       <c r="B90" t="s">
-        <v>161</v>
+        <v>80</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2200,12 +2201,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>107</v>
       </c>
       <c r="B91" t="s">
-        <v>162</v>
+        <v>81</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -2214,12 +2215,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>108</v>
       </c>
       <c r="B92" t="s">
-        <v>163</v>
+        <v>82</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -2228,12 +2229,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>109</v>
       </c>
       <c r="B93" t="s">
-        <v>164</v>
+        <v>83</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -2242,12 +2243,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>110</v>
       </c>
       <c r="B94" t="s">
-        <v>165</v>
+        <v>84</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -2257,6 +2258,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
@@ -2282,21 +2284,21 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>